<commit_message>
Day1 Commit to AWS Study
Day1 Commit to AWS Study
</commit_message>
<xml_diff>
--- a/AWS Interview Q&A.xlsx
+++ b/AWS Interview Q&A.xlsx
@@ -1,62 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Learnings\Interview Q&amp;A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Learnings\Interview Q&amp;A\Interview-Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5564F4E3-377A-489C-8D85-FB5DB89B53AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573F410A-189C-4C44-A84E-7B0D8C4504D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="992" activeTab="7" xr2:uid="{90B1EBA5-1F6D-4829-9F70-A779416569A0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="992" firstSheet="2" activeTab="7" xr2:uid="{90B1EBA5-1F6D-4829-9F70-A779416569A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Basic interview questions" sheetId="24" r:id="rId2"/>
-    <sheet name="VPC" sheetId="11" r:id="rId3"/>
-    <sheet name="EC2" sheetId="3" r:id="rId4"/>
-    <sheet name="SG" sheetId="12" r:id="rId5"/>
-    <sheet name="EC2 Storage" sheetId="25" r:id="rId6"/>
-    <sheet name="IAM" sheetId="6" r:id="rId7"/>
-    <sheet name="S3" sheetId="2" r:id="rId8"/>
-    <sheet name="RDS" sheetId="4" r:id="rId9"/>
-    <sheet name="DMS" sheetId="16" r:id="rId10"/>
-    <sheet name="ELB" sheetId="17" r:id="rId11"/>
-    <sheet name="Encryption" sheetId="5" r:id="rId12"/>
-    <sheet name="Route53" sheetId="19" r:id="rId13"/>
-    <sheet name="CloudTrail" sheetId="18" r:id="rId14"/>
-    <sheet name="Cloudwatch" sheetId="20" r:id="rId15"/>
-    <sheet name="Caching" sheetId="22" r:id="rId16"/>
-    <sheet name="Lambda" sheetId="10" r:id="rId17"/>
-    <sheet name="Athena" sheetId="29" r:id="rId18"/>
-    <sheet name="Kinesis" sheetId="23" r:id="rId19"/>
-    <sheet name="Elastic BeanStalk" sheetId="21" r:id="rId20"/>
-    <sheet name="OpsWorks" sheetId="27" r:id="rId21"/>
-    <sheet name="Configuration Management" sheetId="26" r:id="rId22"/>
-    <sheet name="Communication&amp;Integration" sheetId="28" r:id="rId23"/>
-    <sheet name="CloudFront" sheetId="31" r:id="rId24"/>
-    <sheet name="Sheet2" sheetId="30" r:id="rId25"/>
+    <sheet name="Exam Questions" sheetId="32" r:id="rId3"/>
+    <sheet name="VPC" sheetId="11" r:id="rId4"/>
+    <sheet name="EC2" sheetId="3" r:id="rId5"/>
+    <sheet name="SG" sheetId="12" r:id="rId6"/>
+    <sheet name="EC2 Storage" sheetId="25" r:id="rId7"/>
+    <sheet name="IAM" sheetId="6" r:id="rId8"/>
+    <sheet name="S3" sheetId="2" r:id="rId9"/>
+    <sheet name="RDS" sheetId="4" r:id="rId10"/>
+    <sheet name="DMS" sheetId="16" r:id="rId11"/>
+    <sheet name="ELB" sheetId="17" r:id="rId12"/>
+    <sheet name="Encryption" sheetId="5" r:id="rId13"/>
+    <sheet name="Route53" sheetId="19" r:id="rId14"/>
+    <sheet name="CloudTrail" sheetId="18" r:id="rId15"/>
+    <sheet name="Cloudwatch" sheetId="20" r:id="rId16"/>
+    <sheet name="Caching" sheetId="22" r:id="rId17"/>
+    <sheet name="Lambda" sheetId="10" r:id="rId18"/>
+    <sheet name="Athena" sheetId="29" r:id="rId19"/>
+    <sheet name="Kinesis" sheetId="23" r:id="rId20"/>
+    <sheet name="Elastic BeanStalk" sheetId="21" r:id="rId21"/>
+    <sheet name="OpsWorks" sheetId="27" r:id="rId22"/>
+    <sheet name="Configuration Management" sheetId="26" r:id="rId23"/>
+    <sheet name="Communication&amp;Integration" sheetId="28" r:id="rId24"/>
+    <sheet name="CloudFront" sheetId="31" r:id="rId25"/>
+    <sheet name="Sheet2" sheetId="30" r:id="rId26"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="845">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="877">
   <si>
     <t>S3</t>
   </si>
@@ -3079,12 +3073,125 @@
   <si>
     <t>5 Teraytes</t>
   </si>
+  <si>
+    <t>How to choose an AWS Region?</t>
+  </si>
+  <si>
+    <t>compliance with data governance and legal requirements
+proximity to customers
+available services withiin a region
+pricing which varies from region to region</t>
+  </si>
+  <si>
+    <t>How many Azs each region had</t>
+  </si>
+  <si>
+    <t>usually 3, min 3 max 6</t>
+  </si>
+  <si>
+    <t>How do Azs assure data availability and disaster recovery?</t>
+  </si>
+  <si>
+    <t>Each AZ is onr or more discrete data center with redundant power, networking and connectivity, isolated from the others, connected with high bandwidth ultra low latency networking</t>
+  </si>
+  <si>
+    <t>AWS Points of presence</t>
+  </si>
+  <si>
+    <t>216 PoP(205 Edge locations &amp; 11 regional caches) in 84 cities across 42 countries</t>
+  </si>
+  <si>
+    <t>What are some of the Global aws services?</t>
+  </si>
+  <si>
+    <t>IAM, Doute53, CloudFront, WAF</t>
+  </si>
+  <si>
+    <t>Some of the region specific servcices?</t>
+  </si>
+  <si>
+    <t>EC2(IaaS), Elastic Beanstalk(PaaS), Lambda(FaaS), Rekognition(SaaS)</t>
+  </si>
+  <si>
+    <t>How can you protect your user passwords ?</t>
+  </si>
+  <si>
+    <t>Setup a password policy :
+Set min password length
+require specific character types
+require users to change their pwds after some time(pwd expiratoin)
+allow all IAM users to change their own passwords
+prevent password re-use</t>
+  </si>
+  <si>
+    <t>What is MFA?</t>
+  </si>
+  <si>
+    <t>MFA = password you know + security device you own</t>
+  </si>
+  <si>
+    <t>What are MFA device options in AWS?</t>
+  </si>
+  <si>
+    <t>Virtual Device : Phone only : Google Authenticator &amp; Authy (Multi device),
+Physical device : Universal 2nd Factor(U2F Security Key)
+Hardware key Fob MFA device : Provided by Gemalto (3rd Party)
+Hardware key Fob  MFA Device for AWS GovCloud (US) : Provided by SurePassID(3rd Prty)</t>
+  </si>
+  <si>
+    <t>How do you create a password policy in IAM?</t>
+  </si>
+  <si>
+    <t>Go to IAM -&gt; Account Settings -&gt; Change password policy</t>
+  </si>
+  <si>
+    <t>Click on account -&gt; my security credentials -&gt; MFA -&gt; Activarte MFA -&gt; Virtual MFA device -&gt; Use Authy/Gauthenticator as per need</t>
+  </si>
+  <si>
+    <t>How to setup MFA ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How can users access AWS? </t>
+  </si>
+  <si>
+    <t>AWS management console : protected by password + MFA
+AWS CLI : protected by access keys
+AWS SDK : for code, protected by access keys</t>
+  </si>
+  <si>
+    <t>What are access keys?</t>
+  </si>
+  <si>
+    <t>Secrets like passwords, users manage their own access keys, generated through AWS Console
+Access Key ID : Just like your username
+Secret Access Key : Just like your password</t>
+  </si>
+  <si>
+    <t>Languages supported by AWS SDK</t>
+  </si>
+  <si>
+    <t>Javascript, python, php, .net, ruby, java, go , node.js, c++
+Mobile SDK : Android, iOS
+IoT Device SDK : Embedded C, Arduino</t>
+  </si>
+  <si>
+    <t>How do you create access key for your IAM user?</t>
+  </si>
+  <si>
+    <t>Go to your account user -&gt; IAM -&gt; Users -&gt; Security Credentials -&gt; Create Access Keys</t>
+  </si>
+  <si>
+    <t>How to configure your AWS CLI with access keys?</t>
+  </si>
+  <si>
+    <t>From CLI, enter aws configure -&gt; Enter Access Key ID, Secret Access Key and default region name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3096,6 +3203,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3134,7 +3249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3148,11 +3263,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3460,7 +3576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3482,7 +3598,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I1" t="s">
@@ -3490,10 +3606,10 @@
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
@@ -3504,10 +3620,10 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="J3" t="s">
@@ -3521,7 +3637,7 @@
       <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="8" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="s">
@@ -3532,10 +3648,10 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="J5" t="s">
@@ -3549,7 +3665,7 @@
       <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="J6" t="s">
@@ -3563,7 +3679,7 @@
       <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="8" t="s">
         <v>240</v>
       </c>
       <c r="J7" t="s">
@@ -3577,7 +3693,7 @@
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="8" t="s">
         <v>241</v>
       </c>
       <c r="J8" t="s">
@@ -3588,10 +3704,10 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="6" t="s">
         <v>2</v>
       </c>
       <c r="J9" t="s">
@@ -3602,10 +3718,10 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>242</v>
       </c>
       <c r="K10">
@@ -3647,23 +3763,23 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>692</v>
       </c>
       <c r="C16">
         <v>56</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>693</v>
       </c>
       <c r="C17">
@@ -3683,7 +3799,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>695</v>
       </c>
       <c r="C19">
@@ -3759,7 +3875,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C27">
@@ -3839,6 +3955,323 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E725F8-AB89-4D3D-9211-03C7390556CD}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>738</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="144" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>537</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>560</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>586</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>616</v>
+      </c>
+      <c r="B47" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>741</v>
+      </c>
+      <c r="B49" t="s">
+        <v>742</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAE215C1-8404-4799-B61D-81D9535200BA}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3850,7 +4283,7 @@
   <cols>
     <col min="1" max="1" width="59.21875" customWidth="1"/>
     <col min="2" max="2" width="75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -3935,7 +4368,7 @@
       <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3988,7 +4421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7F8A00-5FCE-4D5D-8D35-9C8424E1AFD9}">
   <dimension ref="A1:B11"/>
   <sheetViews>
@@ -4090,7 +4523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9AE3FC-A732-41DF-85D5-D42FC0451B68}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -4268,7 +4701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF632043-04B2-49CF-83A6-71DBBEE40F5B}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -4447,7 +4880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD63001-C17F-41BE-B67D-30263FF9D66F}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -4474,7 +4907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{253FD0F4-EC0F-4F92-9063-B3ED5A2027D3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -4533,7 +4966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784F6B0B-B46A-45D1-81DF-D36B357B18F5}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -4729,12 +5162,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6547F6-C9E1-44E7-A53B-F6FF9E2734D7}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4750,7 +5183,7 @@
       <c r="B1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>190</v>
       </c>
     </row>
@@ -4761,7 +5194,7 @@
       <c r="B2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>201</v>
       </c>
     </row>
@@ -4972,7 +5405,7 @@
       <c r="B28" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>803</v>
       </c>
     </row>
@@ -4995,7 +5428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{162E598B-71E9-4167-A09D-5FD0F3860387}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5007,12 +5440,102 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE49F43-B642-4DC2-B576-8B2D511B703B}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="53.77734375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>867</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>870</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3C50979-0F54-4FFD-8500-FC805A6D60E4}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5028,7 +5551,7 @@
       <c r="B1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>231</v>
       </c>
     </row>
@@ -5047,7 +5570,7 @@
       <c r="B3" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>222</v>
       </c>
     </row>
@@ -5092,70 +5615,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE49F43-B642-4DC2-B576-8B2D511B703B}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="53.77734375" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF023BF-EC3B-46E0-AD11-E008221D41FB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5193,7 +5658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB30C63-CAE3-4C59-B10B-2F9FFD19FBCA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5205,7 +5670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB3AA015-294D-48CC-8D60-074318C7A04D}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -5245,7 +5710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2FBD861-A55C-48B1-9C84-DFEB9633B360}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -5312,7 +5777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E97398-FA45-4110-9328-8E6DC3B68133}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -5466,7 +5931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7019480-7278-4DCC-A045-61D27E10C90F}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -5479,11 +5944,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7260B819-FE8D-4DFC-8C73-89B4943BD1F9}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="127.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>872</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3860E236-F059-41C7-B425-52E2C1034BE5}">
   <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5993,7 +6517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15524CF-363B-4952-A4D4-9BFF45242465}">
   <dimension ref="A1:C73"/>
   <sheetViews>
@@ -6014,7 +6538,7 @@
       <c r="B1" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>232</v>
       </c>
     </row>
@@ -6565,7 +7089,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A0CB0E-7B1E-4E06-A6C1-6231868AC978}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -6616,7 +7140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3FB4422-27D9-497A-9B26-4CB62121FC34}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -6821,12 +7345,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B1F9BAB-2BB2-4317-BE47-E5D693712C6D}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6932,7 +7456,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>431</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -7043,16 +7567,73 @@
         <v>781</v>
       </c>
     </row>
+    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>857</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>859</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>861</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>863</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>866</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
+        <v>873</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
+        <v>875</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>876</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D5761A-6A3B-4422-86A7-9828FAAFE3C2}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -7222,321 +7803,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E725F8-AB89-4D3D-9211-03C7390556CD}">
-  <dimension ref="A1:B49"/>
-  <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="67" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>738</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>148</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>537</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>560</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>586</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>616</v>
-      </c>
-      <c r="B47" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>741</v>
-      </c>
-      <c r="B49" t="s">
-        <v>742</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>